<commit_message>
modification du diagramme de gant
</commit_message>
<xml_diff>
--- a/diagramme-de-gant.xlsx
+++ b/diagramme-de-gant.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kennedy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kennedy\Desktop\coucou\tpe-SI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="7476" windowHeight="2808"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="7476" windowHeight="2808"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -561,7 +561,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1182,15 +1182,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
+      <xdr:colOff>53340</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1477,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>